<commit_message>
Full multiprocessing support, peak performance
</commit_message>
<xml_diff>
--- a/PlayFair.xlsx
+++ b/PlayFair.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
@@ -771,6 +771,620 @@
         <v>-1403.8837</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>20</v>
+      </c>
+      <c r="B18" t="n">
+        <v>63.56</v>
+      </c>
+      <c r="C18" t="n">
+        <v>12</v>
+      </c>
+      <c r="D18" t="n">
+        <v>300</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8000</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>OPEXUM GCKŁNŻ AĄBĆDĘ FHIJLŃ ÓQRSŚT VWYZŹ|</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>OPEXUM GCKŁNŻ AĄBĆDĘ FHIJLŃ ÓQRSŚT VWYZŹ|</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>24</v>
+      </c>
+      <c r="B19" t="n">
+        <v>82.25</v>
+      </c>
+      <c r="C19" t="n">
+        <v>12</v>
+      </c>
+      <c r="D19" t="n">
+        <v>300</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8000</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>HGZŁJU BSŹAT| ĄCĆDEĘ FIKLMN ŃOÓPQR ŚVWXYŻ</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>HGZŁJU BSŹAT| ĄCĆDEĘ FIKLMN ŃOÓPQR ŚVWXYŻ</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>28</v>
+      </c>
+      <c r="B20" t="n">
+        <v>94.83</v>
+      </c>
+      <c r="C20" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" t="n">
+        <v>300</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8000</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>TDŁFIS NHQ|UK AĄBCĆE ĘGJLMŃ OÓPRŚV WXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>TDŁFIS NHQ|UK AĄBCĆE ĘGJLMŃ OÓPRŚV WXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>11</v>
+      </c>
+      <c r="B21" t="n">
+        <v>28.69</v>
+      </c>
+      <c r="C21" t="n">
+        <v>12</v>
+      </c>
+      <c r="D21" t="n">
+        <v>300</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>VĄŁWŹY LHMIST ABCĆDE ĘFGJKN ŃOÓPQR ŚUXZŻ|</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>VĄŁWŹY LHMIST ABCĆDE ĘFGJKN ŃOÓPQR ŚUXZŻ|</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>35</v>
+      </c>
+      <c r="B22" t="n">
+        <v>72.20999999999999</v>
+      </c>
+      <c r="C22" t="n">
+        <v>12</v>
+      </c>
+      <c r="D22" t="n">
+        <v>300</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>ÓIGUŹC DWĆASK ĄBEĘFH JLŁMNŃ OPQRŚT VXYZŻ|</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ÓIGUŹC DWĆASK ĄBEĘFH JLŁMNŃ OPQRŚT VXYZŻ|</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>68</v>
+      </c>
+      <c r="B23" t="n">
+        <v>150.34</v>
+      </c>
+      <c r="C23" t="n">
+        <v>12</v>
+      </c>
+      <c r="D23" t="n">
+        <v>300</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>ŹĆÓZMI FNWĄX| ABCDEĘ GHJKLŁ ŃOPQRS ŚTUVYŻ</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ŹĆÓZMI FNWĄX| ABCDEĘ GHJKLŁ ŃOPQRS ŚTUVYŻ</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" t="n">
+        <v>47.52</v>
+      </c>
+      <c r="C24" t="n">
+        <v>12</v>
+      </c>
+      <c r="D24" t="n">
+        <v>300</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>AGQDTĘ ŻĆŃC|V ĄBEFHI JKLŁMN OÓPRSŚ UWXYZŹ</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>AGQDTĘ ŻĆŃC|V ĄBEFHI JKLŁMN OÓPRSŚ UWXYZŹ</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>60</v>
+      </c>
+      <c r="B25" t="n">
+        <v>130.68</v>
+      </c>
+      <c r="C25" t="n">
+        <v>12</v>
+      </c>
+      <c r="D25" t="n">
+        <v>300</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N|ŹKŚF JŃMĘCR AĄBĆDE GHILŁO ÓPQSTU VWXYZŻ</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>N|ŹKŚF JŃMĘCR AĄBĆDE GHILŁO ÓPQSTU VWXYZŻ</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>147</v>
+      </c>
+      <c r="B26" t="n">
+        <v>328.28</v>
+      </c>
+      <c r="C26" t="n">
+        <v>12</v>
+      </c>
+      <c r="D26" t="n">
+        <v>300</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ZŹTÓŻQ ĄŚWSOĘ ABCĆDE FGHIJK LŁMNŃP RUVXY|</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ZŹTÓŻQ ĄŚWSOĘ ABCĆDE FGHIJK LŁMNŃP RUVXY|</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>36</v>
+      </c>
+      <c r="B27" t="n">
+        <v>74.14</v>
+      </c>
+      <c r="C27" t="n">
+        <v>12</v>
+      </c>
+      <c r="D27" t="n">
+        <v>300</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>MBNOXS FLVŃGĘ AĄCĆDE HIJKŁÓ PQRŚTU WYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>MBNOXS FLVŃGĘ AĄCĆDE HIJKŁÓ PQRŚTU WYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>52</v>
+      </c>
+      <c r="B28" t="n">
+        <v>106.34</v>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" t="n">
+        <v>300</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ZŃÓTLA OFŚNVM ĄBCĆDE ĘGHIJK ŁPQRSU WXYŹŻ|</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>ZŃÓTLA OFŚNVM ĄBCĆDE ĘGHIJK ŁPQRSU WXYŹŻ|</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>33</v>
+      </c>
+      <c r="B29" t="n">
+        <v>70.59</v>
+      </c>
+      <c r="C29" t="n">
+        <v>12</v>
+      </c>
+      <c r="D29" t="n">
+        <v>300</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>OŹĘŁGZ LMPHŚŻ AĄBCĆD EFIJKN ŃÓQRST UVWXY|</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>OŹĘŁGZ LMPHŚŻ AĄBCĆD EFIJKN ŃÓQRST UVWXY|</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>68</v>
+      </c>
+      <c r="B30" t="n">
+        <v>125.79</v>
+      </c>
+      <c r="C30" t="n">
+        <v>12</v>
+      </c>
+      <c r="D30" t="n">
+        <v>300</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>AWCJQN KUPYIV ĄBĆDEĘ FGHLŁM ŃOÓRSŚ TXZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>AWCJQN KUPYIV ĄBĆDEĘ FGHLŁM ŃOÓRSŚ TXZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>274</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Attempt failed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>274</v>
+      </c>
+      <c r="B32" t="n">
+        <v>643.91</v>
+      </c>
+      <c r="C32" t="n">
+        <v>12</v>
+      </c>
+      <c r="D32" t="n">
+        <v>300</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>AZDŃEQ YLKMPN ĄBCĆĘF GHIJŁO ÓRSŚTU VWXŹŻ|</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>VBJFTŻ UÓRWZS Ź|OMGQ NĄKŚLŁ CAHXDE ŃĘPĆIY</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>-2001.6128</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>20</v>
+      </c>
+      <c r="B33" t="n">
+        <v>46.08</v>
+      </c>
+      <c r="C33" t="n">
+        <v>12</v>
+      </c>
+      <c r="D33" t="n">
+        <v>300</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ŚJŁĆDŹ ĘŻHVFQ AĄBCEG IKLMNŃ OÓPRST UWXYZ|</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>ŚJŁĆDV ĘŻHŹFQ AĄBCEG IKLMNŃ OÓPRST UWXYZ|</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>-1437.7579</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>37</v>
+      </c>
+      <c r="B34" t="n">
+        <v>80.31</v>
+      </c>
+      <c r="C34" t="n">
+        <v>12</v>
+      </c>
+      <c r="D34" t="n">
+        <v>300</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>QONLĆH JCÓSPV AĄBDEĘ FGIKŁM ŃRŚTUW XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>FGIKŁM ŃRŚTUW XYZŹŻ| QONLĆH JCÓSPV AĄBDEĘ</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>255</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Attempt failed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>255</v>
+      </c>
+      <c r="B36" t="n">
+        <v>629.58</v>
+      </c>
+      <c r="C36" t="n">
+        <v>12</v>
+      </c>
+      <c r="D36" t="n">
+        <v>300</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>DKORCŁ I|ĘLHA ĄBĆEFG JMNŃÓP QSŚTUV WXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>ZLTROŃ JCWPŹÓ YGXKŻF QĆMŚBE ADĘNĄH |IVSŁU</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>-1976.7157</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>27</v>
+      </c>
+      <c r="B37" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="C37" t="n">
+        <v>12</v>
+      </c>
+      <c r="D37" t="n">
+        <v>300</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>WŚOS|Ę DKVÓCĆ AĄBEFG HIJLŁM NŃPQRT UXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>WŚOS|Ę DKVÓCĆ AĄBEFG HIJLŁM NŃPQRT UXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="M11:N11"/>

</xml_diff>

<commit_message>
Percent adjustements, better inheritrow
</commit_message>
<xml_diff>
--- a/PlayFair.xlsx
+++ b/PlayFair.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
@@ -2966,6 +2966,501 @@
         <v>-1403.8837</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>26</v>
+      </c>
+      <c r="B88" t="n">
+        <v>66.05</v>
+      </c>
+      <c r="C88" t="n">
+        <v>12</v>
+      </c>
+      <c r="D88" t="n">
+        <v>300</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>HWBAQÓ ŚDJGIŃ ĄCĆEĘF KLŁMNO PRSTUV XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>HWBAQÓ ŚDJGIŃ ĄCĆEĘF KLŁMNO PRSTUV XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>46</v>
+      </c>
+      <c r="B89" t="n">
+        <v>155.07</v>
+      </c>
+      <c r="C89" t="n">
+        <v>12</v>
+      </c>
+      <c r="D89" t="n">
+        <v>300</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>DUZXŚI TĆVSŹA ĄBCEĘF GHJKLŁ MNŃOÓP QRWYŻ|</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>DUZXŚI TĆVSŹA ĄBCEĘF GHJKLŁ MNŃOÓP QRWYŻ|</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>105</v>
+      </c>
+      <c r="B90" t="n">
+        <v>367.03</v>
+      </c>
+      <c r="C90" t="n">
+        <v>12</v>
+      </c>
+      <c r="D90" t="n">
+        <v>300</v>
+      </c>
+      <c r="E90" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>TYIMCJ Ż|ŃĆPN AĄBDEĘ FGHKLŁ OÓQRSŚ UVWXZŹ</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>TYIMCJ Ż|ŃĆPN AĄBDEĘ FGHKLŁ OÓQRSŚ UVWXZŹ</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>15</v>
+      </c>
+      <c r="B91" t="n">
+        <v>53.42</v>
+      </c>
+      <c r="C91" t="n">
+        <v>12</v>
+      </c>
+      <c r="D91" t="n">
+        <v>300</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>JUIRAF ŁNWHZK ĄBCĆDE ĘGLMŃO ÓPQSŚT VXYŹŻ|</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>JUIRAF ŁNWHZK ĄBCĆDE ĘGLMŃO ÓPQSŚT VXYŹŻ|</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>50</v>
+      </c>
+      <c r="B92" t="n">
+        <v>168.1</v>
+      </c>
+      <c r="C92" t="n">
+        <v>12</v>
+      </c>
+      <c r="D92" t="n">
+        <v>300</v>
+      </c>
+      <c r="E92" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>OÓIEŚR ŹBTYLK AĄCĆDĘ FGHJŁM NŃPQSU VWXZŻ|</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>OÓIEŚR ŹBTYLK AĄCĆDĘ FGHJŁM NŃPQSU VWXZŻ|</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>9</v>
+      </c>
+      <c r="B93" t="n">
+        <v>34.72</v>
+      </c>
+      <c r="C93" t="n">
+        <v>12</v>
+      </c>
+      <c r="D93" t="n">
+        <v>300</v>
+      </c>
+      <c r="E93" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>ŹVFCEĄ SYDŃAJ BĆĘGHI KLŁMNO ÓPQRŚT UWXZŻ|</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>ŹVĘCEĄ SYDŃAJ BĆFGHI KLŁMNO ÓPQRŚT UWXZŻ|</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>-1471.1039</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>3</v>
+      </c>
+      <c r="B94" t="n">
+        <v>15.51</v>
+      </c>
+      <c r="C94" t="n">
+        <v>12</v>
+      </c>
+      <c r="D94" t="n">
+        <v>300</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>VŻBTMW FŚXÓRQ AĄCĆDE ĘGHIJK LŁNŃOP SUYZŹ|</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>VŻBTMW FŚXÓRQ AĄCĆDE ĘGHIJK LŁNŃOP SUYZŹ|</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>18</v>
+      </c>
+      <c r="B95" t="n">
+        <v>54.78</v>
+      </c>
+      <c r="C95" t="n">
+        <v>12</v>
+      </c>
+      <c r="D95" t="n">
+        <v>300</v>
+      </c>
+      <c r="E95" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>TŃĘ|ŻŹ FNMAEÓ ĄBCĆDG HIJKLŁ OPQRSŚ UVWXYZ</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>T|ĘŃŻŹ FNMAEÓ ĄBCĆDG HIJKLŁ OPQRSŚ UVWXYZ</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>-1446.2486</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>19</v>
+      </c>
+      <c r="B96" t="n">
+        <v>55.58</v>
+      </c>
+      <c r="C96" t="n">
+        <v>12</v>
+      </c>
+      <c r="D96" t="n">
+        <v>300</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>ŚJŻBĘL KŹINZP AĄCĆDE FGHŁMŃ OÓQRST UVWXY|</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>OÓQRST UVWXY| ŚJŻBĘL KŹINZP AĄCĆDE FGHŁMŃ</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>149</v>
+      </c>
+      <c r="B97" t="n">
+        <v>450.01</v>
+      </c>
+      <c r="C97" t="n">
+        <v>12</v>
+      </c>
+      <c r="D97" t="n">
+        <v>300</v>
+      </c>
+      <c r="E97" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>RGAŃZĘ TPCMŻF ĄBĆDEH IJKLŁN OÓQSŚU VWXYŹ|</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>OÓQSŚU VWXYŹ| RGAŃZĘ TPCMŻF ĄBHDEĆ IJKLŁN</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>-1461.2366</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>15</v>
+      </c>
+      <c r="B98" t="n">
+        <v>46.82</v>
+      </c>
+      <c r="C98" t="n">
+        <v>12</v>
+      </c>
+      <c r="D98" t="n">
+        <v>300</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>ÓUBĄŹŃ MHTYAC ĆDEĘFG IJKLŁN OPQRSŚ VWXZŻ|</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>ÓUŃĄŹB MHTYAC ĆDEĘFG IJKLŁN OPQRSŚ VWXZŻ|</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>-1469.9451</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>13</v>
+      </c>
+      <c r="B99" t="n">
+        <v>43.09</v>
+      </c>
+      <c r="C99" t="n">
+        <v>12</v>
+      </c>
+      <c r="D99" t="n">
+        <v>300</v>
+      </c>
+      <c r="E99" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>VZXGĄB ĆCŚKSF ADEĘHI JLŁMNŃ OÓPQRT UWYŹŻ|</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>VZXGĄB ĆCŚKSF ADEĘHI JLŁMNŃ OÓPQRT UWYŹŻ|</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>21</v>
+      </c>
+      <c r="B100" t="n">
+        <v>95.45999999999999</v>
+      </c>
+      <c r="C100" t="n">
+        <v>12</v>
+      </c>
+      <c r="D100" t="n">
+        <v>300</v>
+      </c>
+      <c r="E100" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>HŃJAŚI LV|OCĘ ĄBĆDEF GKŁMNÓ PQRSTU WXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>HŃJAŚI LV|OCĘ ĄBĆDEF GKŁMNÓ PQRSTU WXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>9</v>
+      </c>
+      <c r="B101" t="n">
+        <v>45.99</v>
+      </c>
+      <c r="C101" t="n">
+        <v>12</v>
+      </c>
+      <c r="D101" t="n">
+        <v>300</v>
+      </c>
+      <c r="E101" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>XŻEŹĘL ŃŚKV|B AĄCĆDF GHIJŁM NOÓPQR STUWYZ</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>XŻEŹĘL ŃŚKV|B AĄCĆDF GHIJŁM NOÓPQR STUWYZ</t>
+        </is>
+      </c>
+      <c r="I101" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>26</v>
+      </c>
+      <c r="B102" t="n">
+        <v>114.93</v>
+      </c>
+      <c r="C102" t="n">
+        <v>12</v>
+      </c>
+      <c r="D102" t="n">
+        <v>300</v>
+      </c>
+      <c r="E102" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>PFJKQO ZÓĄVŚW ABCĆDE ĘGHILŁ MNŃRST UXYŹŻ|</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>PQJKFO ZÓĄVŚW ABCĆDE ĘGHILŁ MNŃRST UXYŹŻ|</t>
+        </is>
+      </c>
+      <c r="I102" t="n">
+        <v>-1450.9253</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="M11:N11"/>

</xml_diff>

<commit_message>
Added plots, currently disabled to improve performance, again adjusted percents of inheritance
</commit_message>
<xml_diff>
--- a/PlayFair.xlsx
+++ b/PlayFair.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:N123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
@@ -3494,6 +3494,756 @@
         <v>-1403.8837</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>13</v>
+      </c>
+      <c r="B104" t="n">
+        <v>63.05</v>
+      </c>
+      <c r="C104" t="n">
+        <v>12</v>
+      </c>
+      <c r="D104" t="n">
+        <v>300</v>
+      </c>
+      <c r="E104" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>QWTMĆU ŚNB|PŁ AĄCDEĘ FGHIJK LŃOÓRS VXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>QWTMĆU ŚNB|PŁ AĄCDEĘ FGHIJK LŃOÓRS VXYZŹŻ</t>
+        </is>
+      </c>
+      <c r="I104" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>31</v>
+      </c>
+      <c r="B105" t="n">
+        <v>136.66</v>
+      </c>
+      <c r="C105" t="n">
+        <v>12</v>
+      </c>
+      <c r="D105" t="n">
+        <v>300</v>
+      </c>
+      <c r="E105" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>ĄXTJGH EZYKŃB ACĆDĘF ILŁMNO ÓPQRSŚ UVWŹŻ|</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>ĄXTJGH EZYKŃB ACĆDĘF ILŁMNO ÓPQRSŚ UVWŹŻ|</t>
+        </is>
+      </c>
+      <c r="I105" t="n">
+        <v>-1403.8837</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>14</v>
+      </c>
+      <c r="B106" t="n">
+        <v>71.45999999999999</v>
+      </c>
+      <c r="C106" t="n">
+        <v>12</v>
+      </c>
+      <c r="D106" t="n">
+        <v>300</v>
+      </c>
+      <c r="E106" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>ĄĘGÓŃQ CVŁXŚO ABĆDEF HIJKLM NPRSTU WYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>WYZŹŻ| ĄĘGÓŃQ ABĆDEF HIJKLM NPRSTU CVŁXŚO</t>
+        </is>
+      </c>
+      <c r="I106" t="n">
+        <v>-1471.5758</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 16:50:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>72</v>
+      </c>
+      <c r="B107" t="n">
+        <v>319.64</v>
+      </c>
+      <c r="C107" t="n">
+        <v>12</v>
+      </c>
+      <c r="D107" t="n">
+        <v>300</v>
+      </c>
+      <c r="E107" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>PVEĄĆQ DJSNUR ABCĘFG HIKLŁM ŃOÓŚTW XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>PVEĄĆQ DJSNUR ABCĘFG HIKLŁM ŃOÓŚTW XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I107" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 16:55:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>16</v>
+      </c>
+      <c r="B108" t="n">
+        <v>109.32</v>
+      </c>
+      <c r="C108" t="n">
+        <v>12</v>
+      </c>
+      <c r="D108" t="n">
+        <v>300</v>
+      </c>
+      <c r="E108" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>DŻXSFU QÓLĘZK AĄBCĆE GHIJŁM NŃOPRŚ TVWYŹ|</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>DŻXSFU QÓLĘZK AĄBCĆE GHIJŁM NŃOPRŚ TVWYŹ|</t>
+        </is>
+      </c>
+      <c r="I108" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:13:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>12</v>
+      </c>
+      <c r="B109" t="n">
+        <v>74.62</v>
+      </c>
+      <c r="C109" t="n">
+        <v>12</v>
+      </c>
+      <c r="D109" t="n">
+        <v>300</v>
+      </c>
+      <c r="E109" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>ĄĘFLÓN ŹJBIŚŁ ACĆDEG HKMŃOP QRSTUV WXYZŻ|</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>ĄĘFLÓN ŹJBIŚŁ ACĆDEG HKMŃOP QRSTUV WXYZŻ|</t>
+        </is>
+      </c>
+      <c r="I109" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:14:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>19</v>
+      </c>
+      <c r="B110" t="n">
+        <v>119.66</v>
+      </c>
+      <c r="C110" t="n">
+        <v>12</v>
+      </c>
+      <c r="D110" t="n">
+        <v>300</v>
+      </c>
+      <c r="E110" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>FYĄMJS ŹOQŃWĆ ABCDEĘ GHIKLŁ NÓPRŚT UVXZŻ|</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>FYĄMJS ŹOQŃWĆ ABCDEĘ GHIKLŁ NÓPRŚT UVXZŻ|</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:16:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>9</v>
+      </c>
+      <c r="B111" t="n">
+        <v>57.42</v>
+      </c>
+      <c r="C111" t="n">
+        <v>12</v>
+      </c>
+      <c r="D111" t="n">
+        <v>300</v>
+      </c>
+      <c r="E111" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>AWŚEVK CÓŁŃGH ĄBĆDĘF IJLMNO PQRSTU XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>AWŚEVK CÓŁŃGH ĄBĆDĘF IJLMNO PQRSTU XYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I111" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:17:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>26</v>
+      </c>
+      <c r="B112" t="n">
+        <v>186.73</v>
+      </c>
+      <c r="C112" t="n">
+        <v>12</v>
+      </c>
+      <c r="D112" t="n">
+        <v>300</v>
+      </c>
+      <c r="E112" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>ÓCVKBM ŃPSYWĄ AĆDEĘF GHIJLŁ NOQRŚT UXZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>ÓCVKBM ŃPSYWĄ AĆDEĘF GHIJLŁ NOQRŚT UXZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I112" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:21:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>36</v>
+      </c>
+      <c r="B113" t="n">
+        <v>232.77</v>
+      </c>
+      <c r="C113" t="n">
+        <v>12</v>
+      </c>
+      <c r="D113" t="n">
+        <v>300</v>
+      </c>
+      <c r="E113" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>HNQŁXS JYKLIĘ AĄBCĆD EFGMŃO ÓPRŚTU VWZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>HNQŁXS JYKLIĘ AĄBCĆD EFGMŃO ÓPRŚTU VWZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I113" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:25:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>10</v>
+      </c>
+      <c r="B114" t="n">
+        <v>66.14</v>
+      </c>
+      <c r="C114" t="n">
+        <v>12</v>
+      </c>
+      <c r="D114" t="n">
+        <v>300</v>
+      </c>
+      <c r="E114" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>EXQĘHA WŃTCRL ĄBĆDFG IJKŁMN OÓPSŚU VYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>EXQĘHA WŃTCRL ĄBĆDFG IJKŁMN OÓPSŚU VYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I114" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:26:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>21</v>
+      </c>
+      <c r="B115" t="n">
+        <v>133.34</v>
+      </c>
+      <c r="C115" t="n">
+        <v>12</v>
+      </c>
+      <c r="D115" t="n">
+        <v>300</v>
+      </c>
+      <c r="E115" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>WFYDHK ŹĘBOPS AĄCĆEG IJLŁMN ŃÓQRŚT UVXZŻ|</t>
+        </is>
+      </c>
+      <c r="G115" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>AĄCĆEG IJLŁMN ŃÓQRŚT UVXZŻ| WFYDHK ŹĘBOPS</t>
+        </is>
+      </c>
+      <c r="I115" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 17:28:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>11</v>
+      </c>
+      <c r="B116" t="n">
+        <v>180.9</v>
+      </c>
+      <c r="C116" t="n">
+        <v>12</v>
+      </c>
+      <c r="D116" t="n">
+        <v>300</v>
+      </c>
+      <c r="E116" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>ŚŹKPCI RULŃSX AĄBĆDE ĘFGHJŁ MNOÓQT VWYZŻ|</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>ŚŹKPCI RULŃSX AĄBĆDE ĘFGHJŁ MNOÓQT VWYZŻ|</t>
+        </is>
+      </c>
+      <c r="I116" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 18:23:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>14</v>
+      </c>
+      <c r="B117" t="n">
+        <v>290.88</v>
+      </c>
+      <c r="C117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D117" t="n">
+        <v>300</v>
+      </c>
+      <c r="E117" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>SŃŻHEĘ I|ĄĆKL ABCDFG JŁMNOÓ PQRŚTU VWXYZŹ</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>SŃŻHEĘ I|ĄĆKL ABCDFG JŁMNOÓ PQRŚTU VWXYZŹ</t>
+        </is>
+      </c>
+      <c r="I117" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 18:30:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>51</v>
+      </c>
+      <c r="B118" t="n">
+        <v>330.99</v>
+      </c>
+      <c r="C118" t="n">
+        <v>12</v>
+      </c>
+      <c r="D118" t="n">
+        <v>300</v>
+      </c>
+      <c r="E118" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>MŹZLIF ŁAEÓCŻ ĄBĆDĘG HJKNŃO PQRSŚT UVWXY|</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>MŹZLIF ŁAEÓCŻ ĄBĆDĘG HJKNŃO PQRSŚT UVWXY|</t>
+        </is>
+      </c>
+      <c r="I118" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 18:48:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>12</v>
+      </c>
+      <c r="B119" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="C119" t="n">
+        <v>12</v>
+      </c>
+      <c r="D119" t="n">
+        <v>300</v>
+      </c>
+      <c r="E119" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>SPMORŃ IX|ĆKB AĄCDEĘ FGHJLŁ NÓQŚTU VWYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>SPMORŃ IX|ĆKB AĄCDEĘ FGHJLŁ NÓQŚTU VWYZŹŻ</t>
+        </is>
+      </c>
+      <c r="I119" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 18:54:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>15</v>
+      </c>
+      <c r="B120" t="n">
+        <v>108.26</v>
+      </c>
+      <c r="C120" t="n">
+        <v>12</v>
+      </c>
+      <c r="D120" t="n">
+        <v>300</v>
+      </c>
+      <c r="E120" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>KĘFPWC ÓNALXV ĄBĆDEG HIJŁMŃ OQRSŚT UYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>KĘFPWC ÓNALXV ĄBĆDEG HIJŁMŃ OQRSŚT UYZŹŻ|</t>
+        </is>
+      </c>
+      <c r="I120" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 18:56:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>51</v>
+      </c>
+      <c r="B121" t="n">
+        <v>357.68</v>
+      </c>
+      <c r="C121" t="n">
+        <v>12</v>
+      </c>
+      <c r="D121" t="n">
+        <v>300</v>
+      </c>
+      <c r="E121" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>IŁNÓUŹ JMCĄAĘ BĆDEFG HKLŃOP QRSŚTV WXYZŻ|</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>IŁNÓUŹ JMCĄAĘ QRSŚTV BĆDEFG HKLŃOP WXYZŻ|</t>
+        </is>
+      </c>
+      <c r="I121" t="n">
+        <v>-1453.0834</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 19:02:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>15</v>
+      </c>
+      <c r="B122" t="n">
+        <v>95.59</v>
+      </c>
+      <c r="C122" t="n">
+        <v>12</v>
+      </c>
+      <c r="D122" t="n">
+        <v>300</v>
+      </c>
+      <c r="E122" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>CŹĄEIG ŁHRPBA ĆDĘFJK LMNŃOÓ QSŚTUV WXYZŻ|</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>CŹĄEIG ŁHRPBA ĆDĘFJK LMNŃOÓ QSŚTUV WXYZŻ|</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 19:04:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>18</v>
+      </c>
+      <c r="B123" t="n">
+        <v>111.65</v>
+      </c>
+      <c r="C123" t="n">
+        <v>12</v>
+      </c>
+      <c r="D123" t="n">
+        <v>300</v>
+      </c>
+      <c r="E123" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>LACXGJ HVÓO|Ć ĄBDEĘF IKŁMNŃ PQRSŚT UWYZŹŻ</t>
+        </is>
+      </c>
+      <c r="G123" t="n">
+        <v>-1403.88365943578</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>LACXGJ HVÓO|Ć ĄBDEĘF IKŁMNŃ PQRSŚT UWYZŹŻ</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
+        <v>-1403.8837</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>30 Jun 2021 19:06:32</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="M11:N11"/>

</xml_diff>